<commit_message>
add conference record by lhw
</commit_message>
<xml_diff>
--- a/doc/讨论记录.xlsx
+++ b/doc/讨论记录.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soft\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12990" windowHeight="6780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,6 +47,14 @@
   </si>
   <si>
     <t>30分钟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>80分钟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>讨论作业要求，确定成员分工，制定计划，分配具体文档、编码工作。介绍github、Travis-ci、word的使用方法</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -387,15 +391,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D9" sqref="D6:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.25" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
@@ -405,14 +410,14 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="81" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>42068.770833333336</v>
       </c>
@@ -424,6 +429,20 @@
       </c>
       <c r="D2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>42069.770833333336</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>